<commit_message>
added an excel List in which one can store all necessarry values
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoga\Documents\Programmieren\Bots\slub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8B92C1-067B-4388-9B1D-ED212C20F947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25658D88-AD21-429F-B6DF-D9D11103385F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{BC03758D-EE5A-4F0E-9926-C3D04F78E838}"/>
+    <workbookView xWindow="0" yWindow="3195" windowWidth="16200" windowHeight="9308" xr2:uid="{BC03758D-EE5A-4F0E-9926-C3D04F78E838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>DATE</t>
   </si>
@@ -75,16 +75,34 @@
   </si>
   <si>
     <t>09:00</t>
+  </si>
+  <si>
+    <t>2025-04-20</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -447,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3CC8D4-D3DF-4200-A602-0D51399F2329}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -516,7 +534,60 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fully functional application, that can automatically make reservations based on an excel sheet
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,116 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yoga\Documents\Programmieren\Bots\slub\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25658D88-AD21-429F-B6DF-D9D11103385F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3195" windowWidth="16200" windowHeight="9308" xr2:uid="{BC03758D-EE5A-4F0E-9926-C3D04F78E838}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>START_TIME</t>
-  </si>
-  <si>
-    <t>END_TIME</t>
-  </si>
-  <si>
-    <t>ROOM_NUMBER</t>
-  </si>
-  <si>
-    <t>LEVEL_NUMBER</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
-    <t>PERSONCOUNT</t>
-  </si>
-  <si>
-    <t>Physik Lerngruppe</t>
-  </si>
-  <si>
-    <t>Erste Verantstaltung</t>
-  </si>
-  <si>
-    <t>2025-04-19</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>2025-04-20</t>
-  </si>
-  <si>
-    <t>11:00</t>
-  </si>
-  <si>
-    <t>14:00</t>
-  </si>
-  <si>
-    <t>2025-04-16</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -129,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -464,130 +440,192 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3CC8D4-D3DF-4200-A602-0D51399F2329}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.9296875" customWidth="1"/>
-    <col min="7" max="7" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col width="9.9296875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.86328125" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="29.33203125" customWidth="1" min="4" max="4"/>
+    <col width="13.59765625" customWidth="1" min="5" max="5"/>
+    <col width="16.9296875" customWidth="1" min="6" max="6"/>
+    <col width="16.53125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="34" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>START_TIME</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>END_TIME</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>ROOM_NUMBERS</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>DESCRIPTION</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>PERSONCOUNT</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>STATUS</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-19</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>0.66|0.46|0.43|0.42|0.47|0.40</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Physik Lerngruppe</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Erste Verantstaltung</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Failed for all Rooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-20</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>08:00</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>09:00</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>0.66|0.46|0.43|0.42|0.47|0.40</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Physik Lerngruppe</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Erste Verantstaltung</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Failed for all Rooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2025-04-16</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>11:00</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>14:00</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>0.66|0.46|0.43|0.42|0.47|0.40</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Physik Lerngruppe</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Erste Verantstaltung</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>6</v>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Success - Reservation for Room 0.46</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>